<commit_message>
Fixed issues with the kpi cumulation
</commit_message>
<xml_diff>
--- a/public/sample_uploads/allocate_account_entries_2/capital_commitments.xlsx
+++ b/public/sample_uploads/allocate_account_entries_2/capital_commitments.xlsx
@@ -497,7 +497,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="45">
   <si>
-    <t xml:space="preserve">Stakeholders *</t>
+    <t xml:space="preserve">Stakeholder *</t>
   </si>
   <si>
     <t xml:space="preserve">Fund *</t>
@@ -1084,7 +1084,7 @@
   <dimension ref="A1:U15"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="false" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.00390625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>